<commit_message>
Actualizacion del archivo de propiedades para segmentar las imagenes de prueba.
</commit_message>
<xml_diff>
--- a/Pruebas/ValidacionOpenComet ES.xlsx
+++ b/Pruebas/ValidacionOpenComet ES.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerardo\Dropbox\INGENIERIA\ENSAYO COMETA\matlab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerardo\Dropbox\INGENIERIA\ENSAYO COMETA\OpenCometUAI_\Pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="68">
   <si>
     <t>OpenComet Original &amp; Modificado</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Edges</t>
   </si>
   <si>
-    <t>ALTERNATIVA ORIGINAL</t>
-  </si>
-  <si>
     <t>ALTERNATIVA MODIFICADO</t>
   </si>
   <si>
@@ -220,13 +217,25 @@
   </si>
   <si>
     <t>CORRECTO</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>OpenComet Modificado</t>
+  </si>
+  <si>
+    <t>Metodo Propuesto</t>
+  </si>
+  <si>
+    <t>Resultado de las pruebas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +277,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00000A"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00000A"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -277,7 +298,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -337,11 +358,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -406,6 +471,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -433,8 +501,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,7 +817,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="I4" sqref="I4:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,22 +834,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="E1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="E1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>32</v>
@@ -759,17 +857,17 @@
       <c r="C2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>32</v>
@@ -791,7 +889,7 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>32</v>
@@ -800,9 +898,9 @@
         <v>20</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="26" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="3">
@@ -816,11 +914,11 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="29"/>
+      <c r="A5" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
       <c r="E5" s="7"/>
       <c r="F5" s="2" t="s">
         <v>3</v>
@@ -837,10 +935,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="24" t="s">
         <v>53</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>54</v>
       </c>
       <c r="C6" s="25">
         <v>400</v>
@@ -853,10 +951,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="25">
         <v>0.85</v>
@@ -879,10 +977,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="25">
         <v>0.5</v>
@@ -903,10 +1001,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="25">
         <v>1.05</v>
@@ -918,11 +1016,11 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
+      <c r="A10" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
       <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
@@ -939,10 +1037,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" s="25">
         <v>0.15</v>
@@ -966,10 +1064,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="25">
         <v>0.2</v>
@@ -992,15 +1090,15 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="29"/>
+      <c r="A13" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="24" t="s">
         <v>32</v>
@@ -1025,10 +1123,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,44 +1135,46 @@
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.5703125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="16" customWidth="1"/>
     <col min="6" max="6" width="2" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" style="16" customWidth="1"/>
     <col min="8" max="8" width="2.42578125" customWidth="1"/>
     <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.85546875" customWidth="1"/>
-    <col min="15" max="15" width="68.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="3.85546875" customWidth="1"/>
+    <col min="16" max="16" width="68.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:16" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
       <c r="D1" s="20"/>
-      <c r="E1" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="E1" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
       <c r="H1" s="18"/>
-      <c r="I1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="6"/>
-      <c r="O1" s="10"/>
-    </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I1" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="38"/>
+      <c r="P1" s="10"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>32</v>
@@ -1084,27 +1184,30 @@
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>32</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="H2" s="8"/>
-      <c r="I2" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="O2" s="10"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I2" s="43"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" s="42"/>
+      <c r="M2" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="N2" s="40"/>
+      <c r="P2" s="10"/>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>32</v>
@@ -1114,7 +1217,7 @@
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>32</v>
@@ -1123,22 +1226,25 @@
         <v>31</v>
       </c>
       <c r="H3" s="8"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="O3" s="10"/>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="10"/>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>32</v>
@@ -1148,13 +1254,13 @@
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>32</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="7" t="s">
@@ -1164,61 +1270,67 @@
         <v>1</v>
       </c>
       <c r="K4" s="3">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="L4" s="3">
         <v>19</v>
       </c>
       <c r="M4" s="3">
+        <v>10</v>
+      </c>
+      <c r="N4" s="3">
         <v>19</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="P4" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="29"/>
+    <row r="5" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29"/>
+      <c r="E5" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="29"/>
+      <c r="G5" s="30"/>
       <c r="H5" s="18"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="2">
         <v>0</v>
       </c>
       <c r="L5" s="2">
         <v>0</v>
       </c>
       <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
         <v>1</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="P5" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="2">
-        <v>400</v>
+      <c r="C6" s="4">
+        <v>3000</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>33</v>
@@ -1229,24 +1341,25 @@
       <c r="H6" s="8"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="4"/>
+      <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="O6" s="12"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N6" s="2"/>
+      <c r="P6" s="12"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="2">
-        <v>0.85</v>
+      <c r="C7" s="4">
+        <v>0.5</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>33</v>
@@ -1261,114 +1374,126 @@
       <c r="J7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="4">
-        <v>84</v>
+      <c r="K7" s="2">
+        <v>5</v>
       </c>
       <c r="L7" s="2">
         <v>1</v>
       </c>
       <c r="M7" s="2">
+        <v>12</v>
+      </c>
+      <c r="N7" s="2">
         <v>1</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="P7" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="4">
         <v>0.5</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>34</v>
       </c>
       <c r="G8" s="4">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="7"/>
       <c r="J8" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="4">
-        <v>11</v>
+      <c r="K8" s="14">
+        <v>2</v>
       </c>
       <c r="L8" s="14">
         <v>1</v>
       </c>
       <c r="M8" s="14">
+        <v>10</v>
+      </c>
+      <c r="N8" s="14">
         <v>1</v>
       </c>
-      <c r="O8" s="13" t="s">
+      <c r="P8" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="4">
         <v>1.05</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>34</v>
       </c>
       <c r="G9" s="4">
-        <v>1.05</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="4"/>
+      <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="O9" s="8"/>
-    </row>
-    <row r="10" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
+      <c r="N9" s="2"/>
+      <c r="P9" s="8"/>
+    </row>
+    <row r="10" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="20"/>
-      <c r="E10" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="29"/>
+      <c r="E10" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="29"/>
+      <c r="G10" s="30"/>
       <c r="H10" s="18"/>
       <c r="I10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="J10" s="7"/>
-      <c r="K10" s="4">
+      <c r="K10" s="2">
         <v>20</v>
       </c>
       <c r="L10" s="2">
         <v>20</v>
       </c>
-      <c r="M10" s="2"/>
-      <c r="O10" s="8"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M10" s="2">
+        <v>20</v>
+      </c>
+      <c r="N10" s="2">
+        <v>20</v>
+      </c>
+      <c r="P10" s="8"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>34</v>
@@ -1378,13 +1503,13 @@
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="4">
-        <v>0.15</v>
+      <c r="G11" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="2" t="s">
@@ -1392,22 +1517,26 @@
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="15">
-        <f>((100*K4)/(K4+K8))</f>
-        <v>45</v>
+        <f t="shared" ref="K11" si="0">((100*K4)/(K4+K8))</f>
+        <v>90</v>
       </c>
       <c r="L11" s="15">
-        <f t="shared" ref="L11:M11" si="0">((100*L4)/(L4+L8))</f>
+        <f>((100*L4)/(L4+L8))</f>
         <v>95</v>
       </c>
       <c r="M11" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="M11" si="1">((100*M4)/(M4+M8))</f>
+        <v>50</v>
+      </c>
+      <c r="N11" s="15">
+        <f t="shared" ref="N11" si="2">((100*N4)/(N4+N8))</f>
         <v>95</v>
       </c>
-      <c r="O11" s="8"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" s="8"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>34</v>
@@ -1417,13 +1546,13 @@
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="4">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="14" t="s">
@@ -1431,37 +1560,41 @@
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="15">
-        <f>((100*K5)/(K5+K7))</f>
+        <f t="shared" ref="K12" si="3">((100*K5)/(K5+K7))</f>
         <v>0</v>
       </c>
       <c r="L12" s="15">
-        <f t="shared" ref="L12:M12" si="1">((100*L5)/(L5+L7))</f>
+        <f>((100*L5)/(L5+L7))</f>
         <v>0</v>
       </c>
       <c r="M12" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="M12" si="4">((100*M5)/(M5+M7))</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="15">
+        <f t="shared" ref="N12" si="5">((100*N5)/(N5+N7))</f>
         <v>50</v>
       </c>
-      <c r="O12" s="8"/>
-    </row>
-    <row r="13" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="P12" s="8"/>
+    </row>
+    <row r="13" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="29"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="19"/>
+      <c r="P13" s="8"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
         <v>48</v>
-      </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="19"/>
-      <c r="O13" s="8"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
-        <v>49</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>32</v>
@@ -1471,7 +1604,7 @@
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>32</v>
@@ -1480,265 +1613,153 @@
         <v>31</v>
       </c>
       <c r="H14" s="8"/>
-      <c r="O14" s="8"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O15" s="8"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
+      <c r="P14" s="8"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P15" s="8"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
-      <c r="O16" s="8"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="P16" s="8"/>
+    </row>
+    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D17" s="9"/>
       <c r="E17" s="20"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
-      <c r="O17" s="8"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="P17" s="8"/>
+    </row>
+    <row r="18" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D18" s="9"/>
       <c r="E18" s="20"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
-      <c r="O18" s="8"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>59</v>
-      </c>
+      <c r="P18" s="8"/>
+    </row>
+    <row r="19" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D19" s="9"/>
       <c r="E19" s="20"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
-      <c r="O19" s="8"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="29"/>
+      <c r="P19" s="8"/>
+    </row>
+    <row r="20" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
-      <c r="O20" s="8"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="4">
-        <v>3000</v>
-      </c>
+      <c r="P20" s="8"/>
+    </row>
+    <row r="21" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D21" s="9"/>
       <c r="E21" s="20"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
-      <c r="O21" s="8"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="4">
-        <v>0.5</v>
-      </c>
+      <c r="P21" s="8"/>
+    </row>
+    <row r="22" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D22" s="9"/>
       <c r="E22" s="20"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
-      <c r="O22" s="8"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="4">
-        <v>0.7</v>
-      </c>
+      <c r="P22" s="8"/>
+    </row>
+    <row r="23" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D23" s="9"/>
       <c r="E23" s="20"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="O23" s="8"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="4">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="P23" s="8"/>
+    </row>
+    <row r="24" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
-      <c r="O24" s="8"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="29"/>
+      <c r="P24" s="8"/>
+    </row>
+    <row r="25" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
       <c r="G25" s="20"/>
-      <c r="O25" s="8"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="P25" s="8"/>
+    </row>
+    <row r="26" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-      <c r="O26" s="8"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="4">
-        <v>0.1</v>
-      </c>
+      <c r="P26" s="8"/>
+    </row>
+    <row r="27" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-      <c r="O27" s="8"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="29"/>
+      <c r="P27" s="8"/>
+    </row>
+    <row r="28" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
-      <c r="O28" s="8"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="P28" s="8"/>
+    </row>
+    <row r="29" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="O29" s="8"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O30" s="8"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O31" s="8"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O32" s="8"/>
-    </row>
-    <row r="33" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O33" s="8"/>
-    </row>
-    <row r="34" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O34" s="8"/>
-    </row>
-    <row r="35" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O35" s="8"/>
-    </row>
-    <row r="36" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O36" s="8"/>
-    </row>
-    <row r="37" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O37" s="8"/>
-    </row>
-    <row r="38" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O38" s="8"/>
-    </row>
-    <row r="39" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O39" s="8"/>
+      <c r="P29" s="8"/>
+    </row>
+    <row r="30" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="P30" s="8"/>
+    </row>
+    <row r="31" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="P31" s="8"/>
+    </row>
+    <row r="32" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="P32" s="8"/>
+    </row>
+    <row r="33" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P33" s="8"/>
+    </row>
+    <row r="34" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P34" s="8"/>
+    </row>
+    <row r="35" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P35" s="8"/>
+    </row>
+    <row r="36" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P36" s="8"/>
+    </row>
+    <row r="37" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P37" s="8"/>
+    </row>
+    <row r="38" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P38" s="8"/>
+    </row>
+    <row r="39" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P39" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A28:C28"/>
+  <mergeCells count="12">
     <mergeCell ref="A13:C13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="I2:M2"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A10:C10"/>
+    <mergeCell ref="E1:G1"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="I2:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1767,17 +1788,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="E1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="A1" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="E1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1790,13 +1811,13 @@
       <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1826,7 +1847,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>2</v>
@@ -1843,11 +1864,11 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
       <c r="E5" s="7"/>
       <c r="F5" s="2" t="s">
         <v>3</v>
@@ -1939,11 +1960,11 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
       <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
@@ -2005,11 +2026,11 @@
       <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -2057,17 +2078,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="E1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="A1" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="E1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2080,13 +2101,13 @@
       <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2116,7 +2137,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
@@ -2133,11 +2154,11 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
         <v>3</v>
@@ -2229,11 +2250,11 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
       <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
@@ -2295,11 +2316,11 @@
       <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -2347,17 +2368,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="E1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="A1" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="E1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2370,13 +2391,13 @@
       <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2423,11 +2444,11 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
         <v>3</v>
@@ -2519,11 +2540,11 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
       <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
@@ -2585,11 +2606,11 @@
       <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -2637,17 +2658,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="E1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="A1" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="E1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2660,13 +2681,13 @@
       <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2696,7 +2717,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
@@ -2713,11 +2734,11 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
         <v>3</v>
@@ -2809,11 +2830,11 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
       <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
@@ -2875,11 +2896,11 @@
       <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -2927,17 +2948,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="E1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="A1" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="E1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2950,13 +2971,13 @@
       <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2986,7 +3007,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2</v>
@@ -3003,11 +3024,11 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
         <v>3</v>
@@ -3099,11 +3120,11 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
       <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
@@ -3165,11 +3186,11 @@
       <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">

</xml_diff>